<commit_message>
Added in previous lab MATLAB files and more excel sheets for lab 6
</commit_message>
<xml_diff>
--- a/Cog Sci 242 F17 Lab 6 - Regression Analysis.xlsx
+++ b/Cog Sci 242 F17 Lab 6 - Regression Analysis.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knoerr/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanessa5\Google Drive\Oxy 2018 Fall\CogS 242\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8D7A1B2B-83ED-6C49-85B4-1A03C2E6CCE6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F807D36-5D55-491C-892A-8339623C83DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1340" windowWidth="25280" windowHeight="13520" activeTab="1"/>
+    <workbookView xWindow="1320" yWindow="1343" windowWidth="25283" windowHeight="13523" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="15" r:id="rId1"/>
     <sheet name="Least Squares Linear Regression" sheetId="13" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -419,9 +426,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -802,21 +809,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -2245,7 +2252,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2289,7 +2296,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2310,28 +2317,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="3.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.46484375" customWidth="1"/>
+    <col min="6" max="6" width="3.1328125" customWidth="1"/>
     <col min="8" max="8" width="2.33203125" customWidth="1"/>
     <col min="9" max="9" width="6.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="9.46484375" customWidth="1"/>
     <col min="11" max="11" width="7.6640625" customWidth="1"/>
-    <col min="12" max="12" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="8.46484375" customWidth="1"/>
     <col min="13" max="13" width="7.6640625" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -2339,7 +2346,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="G2" s="50"/>
       <c r="H2" s="50"/>
       <c r="I2" s="48"/>
@@ -2354,7 +2361,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -2394,7 +2401,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>51</v>
       </c>
@@ -2422,7 +2429,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>52</v>
       </c>
@@ -2450,7 +2457,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>60</v>
       </c>
@@ -2478,7 +2485,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>67</v>
       </c>
@@ -2506,7 +2513,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>69</v>
       </c>
@@ -2534,7 +2541,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>71</v>
       </c>
@@ -2562,7 +2569,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>76</v>
       </c>
@@ -2590,7 +2597,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>78</v>
       </c>
@@ -2637,7 +2644,7 @@
         <v>420.75</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>50</v>
       </c>
@@ -2665,7 +2672,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>57</v>
       </c>
@@ -2693,7 +2700,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>58</v>
       </c>
@@ -2721,7 +2728,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>63</v>
       </c>
@@ -2749,7 +2756,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>75</v>
       </c>
@@ -2777,7 +2784,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>77</v>
       </c>
@@ -2805,7 +2812,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>79</v>
       </c>
@@ -2833,7 +2840,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>80</v>
       </c>
@@ -2880,7 +2887,7 @@
         <v>456.5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>53</v>
       </c>
@@ -2908,7 +2915,7 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>61</v>
       </c>
@@ -2936,7 +2943,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>66</v>
       </c>
@@ -2964,7 +2971,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>73</v>
       </c>
@@ -2992,7 +2999,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>74</v>
       </c>
@@ -3020,7 +3027,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>85</v>
       </c>
@@ -3048,7 +3055,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>93</v>
       </c>
@@ -3076,7 +3083,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>95</v>
       </c>
@@ -3123,7 +3130,7 @@
         <v>1095.25</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>64</v>
       </c>
@@ -3151,7 +3158,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>81</v>
       </c>
@@ -3179,7 +3186,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>82</v>
       </c>
@@ -3207,7 +3214,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>84</v>
       </c>
@@ -3235,7 +3242,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>87</v>
       </c>
@@ -3263,7 +3270,7 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>88</v>
       </c>
@@ -3291,7 +3298,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>91</v>
       </c>
@@ -3319,7 +3326,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>92</v>
       </c>
@@ -3366,7 +3373,7 @@
         <v>210.25</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>49</v>
       </c>
@@ -3394,7 +3401,7 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>55</v>
       </c>
@@ -3422,7 +3429,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>59</v>
       </c>
@@ -3450,7 +3457,7 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>65</v>
       </c>
@@ -3478,7 +3485,7 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>68</v>
       </c>
@@ -3506,7 +3513,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>70</v>
       </c>
@@ -3534,7 +3541,7 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>86</v>
       </c>
@@ -3562,7 +3569,7 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>90</v>
       </c>
@@ -3609,7 +3616,7 @@
         <v>156.25</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>54</v>
       </c>
@@ -3637,7 +3644,7 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>56</v>
       </c>
@@ -3665,7 +3672,7 @@
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>62</v>
       </c>
@@ -3693,7 +3700,7 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>72</v>
       </c>
@@ -3721,7 +3728,7 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>83</v>
       </c>
@@ -3749,7 +3756,7 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>89</v>
       </c>
@@ -3777,7 +3784,7 @@
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>94</v>
       </c>
@@ -3805,7 +3812,7 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>96</v>
       </c>
@@ -3852,7 +3859,7 @@
         <v>639.5</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>2</v>
       </c>
@@ -3880,7 +3887,7 @@
       <c r="N52" s="69"/>
       <c r="O52" s="69"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>15</v>
       </c>
@@ -3908,7 +3915,7 @@
       <c r="N53" s="69"/>
       <c r="O53" s="69"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>17</v>
       </c>
@@ -3936,7 +3943,7 @@
       <c r="N54" s="69"/>
       <c r="O54" s="69"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>20</v>
       </c>
@@ -3964,7 +3971,7 @@
       <c r="N55" s="69"/>
       <c r="O55" s="69"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>22</v>
       </c>
@@ -3992,7 +3999,7 @@
       <c r="N56" s="69"/>
       <c r="O56" s="69"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>33</v>
       </c>
@@ -4020,7 +4027,7 @@
       <c r="N57" s="69"/>
       <c r="O57" s="69"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>36</v>
       </c>
@@ -4048,7 +4055,7 @@
       <c r="N58" s="69"/>
       <c r="O58" s="69"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>46</v>
       </c>
@@ -4095,7 +4102,7 @@
         <v>73.75</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>16</v>
       </c>
@@ -4123,7 +4130,7 @@
       <c r="N60" s="69"/>
       <c r="O60" s="69"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>21</v>
       </c>
@@ -4151,7 +4158,7 @@
       <c r="N61" s="69"/>
       <c r="O61" s="69"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>23</v>
       </c>
@@ -4179,7 +4186,7 @@
       <c r="N62" s="69"/>
       <c r="O62" s="69"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>25</v>
       </c>
@@ -4207,7 +4214,7 @@
       <c r="N63" s="69"/>
       <c r="O63" s="69"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>30</v>
       </c>
@@ -4235,7 +4242,7 @@
       <c r="N64" s="69"/>
       <c r="O64" s="69"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>37</v>
       </c>
@@ -4263,7 +4270,7 @@
       <c r="N65" s="69"/>
       <c r="O65" s="69"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>40</v>
       </c>
@@ -4291,7 +4298,7 @@
       <c r="N66" s="69"/>
       <c r="O66" s="69"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>45</v>
       </c>
@@ -4338,7 +4345,7 @@
         <v>143.75</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>1</v>
       </c>
@@ -4366,7 +4373,7 @@
       <c r="N68" s="69"/>
       <c r="O68" s="69"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>8</v>
       </c>
@@ -4394,7 +4401,7 @@
       <c r="N69" s="69"/>
       <c r="O69" s="69"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>18</v>
       </c>
@@ -4422,7 +4429,7 @@
       <c r="N70" s="69"/>
       <c r="O70" s="69"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>27</v>
       </c>
@@ -4450,7 +4457,7 @@
       <c r="N71" s="69"/>
       <c r="O71" s="69"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>28</v>
       </c>
@@ -4478,7 +4485,7 @@
       <c r="N72" s="69"/>
       <c r="O72" s="69"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>34</v>
       </c>
@@ -4506,7 +4513,7 @@
       <c r="N73" s="69"/>
       <c r="O73" s="69"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>39</v>
       </c>
@@ -4534,7 +4541,7 @@
       <c r="N74" s="69"/>
       <c r="O74" s="69"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>44</v>
       </c>
@@ -4581,7 +4588,7 @@
         <v>121.25</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>3</v>
       </c>
@@ -4609,7 +4616,7 @@
       <c r="N76" s="69"/>
       <c r="O76" s="69"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>12</v>
       </c>
@@ -4637,7 +4644,7 @@
       <c r="N77" s="69"/>
       <c r="O77" s="69"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>13</v>
       </c>
@@ -4665,7 +4672,7 @@
       <c r="N78" s="69"/>
       <c r="O78" s="69"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>32</v>
       </c>
@@ -4693,7 +4700,7 @@
       <c r="N79" s="69"/>
       <c r="O79" s="69"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>35</v>
       </c>
@@ -4721,7 +4728,7 @@
       <c r="N80" s="69"/>
       <c r="O80" s="69"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>41</v>
       </c>
@@ -4749,7 +4756,7 @@
       <c r="N81" s="69"/>
       <c r="O81" s="69"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>42</v>
       </c>
@@ -4777,7 +4784,7 @@
       <c r="N82" s="69"/>
       <c r="O82" s="69"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>48</v>
       </c>
@@ -4824,7 +4831,7 @@
         <v>120.25</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>4</v>
       </c>
@@ -4852,7 +4859,7 @@
       <c r="N84" s="69"/>
       <c r="O84" s="69"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>5</v>
       </c>
@@ -4880,7 +4887,7 @@
       <c r="N85" s="69"/>
       <c r="O85" s="69"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>9</v>
       </c>
@@ -4908,7 +4915,7 @@
       <c r="N86" s="69"/>
       <c r="O86" s="69"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>14</v>
       </c>
@@ -4936,7 +4943,7 @@
       <c r="N87" s="69"/>
       <c r="O87" s="69"/>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>24</v>
       </c>
@@ -4964,7 +4971,7 @@
       <c r="N88" s="69"/>
       <c r="O88" s="69"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>31</v>
       </c>
@@ -4992,7 +4999,7 @@
       <c r="N89" s="69"/>
       <c r="O89" s="69"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>38</v>
       </c>
@@ -5020,7 +5027,7 @@
       <c r="N90" s="69"/>
       <c r="O90" s="69"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>47</v>
       </c>
@@ -5067,7 +5074,7 @@
         <v>108.25</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>6</v>
       </c>
@@ -5095,7 +5102,7 @@
       <c r="N92" s="69"/>
       <c r="O92" s="69"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>7</v>
       </c>
@@ -5123,7 +5130,7 @@
       <c r="N93" s="69"/>
       <c r="O93" s="69"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>10</v>
       </c>
@@ -5151,7 +5158,7 @@
       <c r="N94" s="69"/>
       <c r="O94" s="69"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>11</v>
       </c>
@@ -5179,7 +5186,7 @@
       <c r="N95" s="69"/>
       <c r="O95" s="69"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>19</v>
       </c>
@@ -5207,7 +5214,7 @@
       <c r="N96" s="69"/>
       <c r="O96" s="69"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>26</v>
       </c>
@@ -5235,7 +5242,7 @@
       <c r="N97" s="69"/>
       <c r="O97" s="69"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>29</v>
       </c>
@@ -5256,7 +5263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>43</v>
       </c>
@@ -5312,34 +5319,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.46484375" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.796875" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.796875" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="10.46484375" customWidth="1"/>
     <col min="13" max="14" width="10.6640625" customWidth="1"/>
     <col min="15" max="15" width="11.33203125" customWidth="1"/>
     <col min="16" max="16" width="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5" customWidth="1"/>
-    <col min="18" max="18" width="11.5" customWidth="1"/>
+    <col min="17" max="17" width="10.46484375" customWidth="1"/>
+    <col min="18" max="18" width="11.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -5348,11 +5355,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="34"/>
       <c r="B3" s="22" t="s">
         <v>29</v>
@@ -5377,7 +5384,7 @@
       <c r="R3" s="54"/>
       <c r="S3" s="55"/>
     </row>
-    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="C4" s="2"/>
       <c r="K4" s="56"/>
@@ -5396,7 +5403,7 @@
       </c>
       <c r="S4" s="65"/>
     </row>
-    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="16" t="s">
         <v>46</v>
@@ -5440,7 +5447,7 @@
       </c>
       <c r="S5" s="65"/>
     </row>
-    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
@@ -5464,7 +5471,7 @@
       <c r="R6" s="68"/>
       <c r="S6" s="65"/>
     </row>
-    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="C7" s="28" t="s">
         <v>27</v>
@@ -5502,7 +5509,7 @@
       <c r="R7" s="68"/>
       <c r="S7" s="65"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="C8" s="28"/>
       <c r="D8" s="35"/>
       <c r="E8" s="28"/>
@@ -5523,7 +5530,7 @@
       <c r="R8" s="68"/>
       <c r="S8" s="65"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -5547,7 +5554,7 @@
       <c r="R9" s="68"/>
       <c r="S9" s="65"/>
     </row>
-    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="67">
         <f>MAX(A14:A68)</f>
         <v>24</v>
@@ -5577,7 +5584,7 @@
       <c r="R10" s="58"/>
       <c r="S10" s="59"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="17" t="s">
         <v>23</v>
@@ -5587,7 +5594,7 @@
       </c>
       <c r="D11" s="33"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="17" t="s">
         <v>22</v>
@@ -5614,7 +5621,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
         <v>2</v>
       </c>
@@ -5643,7 +5650,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10">
         <f>IF(COUNTBLANK(C14)=0,1,0)</f>
         <v>1</v>
@@ -5685,7 +5692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <f>IF(COUNTBLANK(C15)=0,A14+1,A14)</f>
         <v>2</v>
@@ -5729,7 +5736,7 @@
         <v>4244</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A16" s="10">
         <f t="shared" ref="A16:A37" si="6">IF(COUNTBLANK(C16)=0,A15+1,A15)</f>
         <v>3</v>
@@ -5776,7 +5783,7 @@
         <v>3932</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -5823,7 +5830,7 @@
         <v>5116</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -5867,7 +5874,7 @@
         <v>9488</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -5911,7 +5918,7 @@
         <v>3496</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -5955,7 +5962,7 @@
         <v>4620</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -5999,7 +6006,7 @@
         <v>6676</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -6043,7 +6050,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -6087,7 +6094,7 @@
         <v>28208</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -6131,7 +6138,7 @@
         <v>29456</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -6175,7 +6182,7 @@
         <v>30704</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <f t="shared" si="6"/>
         <v>13</v>
@@ -6219,7 +6226,7 @@
         <v>22704</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <f t="shared" si="6"/>
         <v>14</v>
@@ -6263,7 +6270,7 @@
         <v>27456</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -6307,7 +6314,7 @@
         <v>21712</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="10">
         <f t="shared" si="6"/>
         <v>16</v>
@@ -6355,7 +6362,7 @@
         <v>18208</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <f t="shared" si="6"/>
         <v>17</v>
@@ -6403,7 +6410,7 @@
         <v>19728</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <f t="shared" si="6"/>
         <v>18</v>
@@ -6447,7 +6454,7 @@
         <v>183680</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <f t="shared" si="6"/>
         <v>19</v>
@@ -6491,7 +6498,7 @@
         <v>260608</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <f t="shared" si="6"/>
         <v>20</v>
@@ -6535,7 +6542,7 @@
         <v>172736</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="10">
         <f t="shared" si="6"/>
         <v>21</v>
@@ -6579,7 +6586,7 @@
         <v>162688</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
         <f t="shared" si="6"/>
         <v>22</v>
@@ -6623,7 +6630,7 @@
         <v>135808</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="10">
         <f t="shared" si="6"/>
         <v>23</v>
@@ -6667,7 +6674,7 @@
         <v>122816</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <f t="shared" si="6"/>
         <v>24</v>
@@ -6711,7 +6718,7 @@
         <v>123840</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="10"/>
       <c r="B38" s="25"/>
       <c r="C38" s="6"/>
@@ -6730,7 +6737,7 @@
         <v>324480</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="10"/>
       <c r="B39" s="25"/>
       <c r="C39" s="6"/>
@@ -6749,7 +6756,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="10"/>
       <c r="B40" s="25"/>
       <c r="C40" s="6"/>
@@ -6768,7 +6775,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
       <c r="B41" s="25"/>
       <c r="C41" s="6"/>
@@ -6787,7 +6794,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="10"/>
       <c r="B42" s="25"/>
       <c r="C42" s="6"/>
@@ -6806,7 +6813,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="10"/>
       <c r="B43" s="25"/>
       <c r="C43" s="6"/>
@@ -6825,7 +6832,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="10"/>
       <c r="B44" s="25"/>
       <c r="C44" s="6"/>
@@ -6844,7 +6851,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="10"/>
       <c r="B45" s="25"/>
       <c r="C45" s="6"/>
@@ -6863,7 +6870,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="10"/>
       <c r="B46" s="25"/>
       <c r="C46" s="6"/>
@@ -6882,7 +6889,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="10"/>
       <c r="B47" s="25"/>
       <c r="C47" s="6"/>
@@ -6901,7 +6908,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="10"/>
       <c r="B48" s="25"/>
       <c r="C48" s="6"/>
@@ -6920,7 +6927,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="10"/>
       <c r="B49" s="25"/>
       <c r="C49" s="6"/>
@@ -6939,7 +6946,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="10"/>
       <c r="B50" s="25"/>
       <c r="C50" s="6"/>
@@ -6958,7 +6965,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="10"/>
       <c r="B51" s="25"/>
       <c r="C51" s="6"/>
@@ -6977,7 +6984,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="10"/>
       <c r="B52" s="25"/>
       <c r="C52" s="6"/>
@@ -6996,7 +7003,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="10"/>
       <c r="B53" s="25"/>
       <c r="C53" s="6"/>
@@ -7015,7 +7022,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
       <c r="B54" s="25"/>
       <c r="C54" s="6"/>
@@ -7034,7 +7041,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="10"/>
       <c r="B55" s="25"/>
       <c r="C55" s="6"/>
@@ -7053,7 +7060,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="10"/>
       <c r="B56" s="25"/>
       <c r="C56" s="6"/>
@@ -7072,7 +7079,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="10"/>
       <c r="B57" s="25"/>
       <c r="C57" s="6"/>
@@ -7091,7 +7098,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="10"/>
       <c r="B58" s="25"/>
       <c r="C58" s="6"/>
@@ -7110,7 +7117,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="10"/>
       <c r="B59" s="25"/>
       <c r="C59" s="6"/>
@@ -7129,7 +7136,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="10"/>
       <c r="B60" s="25"/>
       <c r="C60" s="6"/>
@@ -7148,7 +7155,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="10"/>
       <c r="B61" s="25"/>
       <c r="C61" s="6"/>
@@ -7167,7 +7174,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="10"/>
       <c r="B62" s="25"/>
       <c r="C62" s="6"/>
@@ -7186,7 +7193,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="10"/>
       <c r="B63" s="25"/>
       <c r="C63" s="6"/>
@@ -7205,7 +7212,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="10"/>
       <c r="B64" s="25"/>
       <c r="C64" s="6"/>
@@ -7224,7 +7231,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" s="10"/>
       <c r="B65" s="25"/>
       <c r="C65" s="6"/>
@@ -7243,7 +7250,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="10"/>
       <c r="B66" s="25"/>
       <c r="C66" s="6"/>
@@ -7262,7 +7269,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="10"/>
       <c r="B67" s="25"/>
       <c r="C67" s="6"/>
@@ -7281,7 +7288,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" s="10"/>
       <c r="B68" s="25"/>
       <c r="C68" s="6"/>
@@ -7300,7 +7307,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="R69" s="3" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -7310,15 +7317,15 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="R70" s="3"/>
       <c r="S70" s="3"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="R71" s="3"/>
       <c r="S71" s="3"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="R72" s="3"/>
       <c r="S72" s="3"/>
     </row>

</xml_diff>